<commit_message>
update simulation for building measurment instrument of learning outcomes
</commit_message>
<xml_diff>
--- a/study03/report/correlation/effective-participants/SimpleCorrPairAnalysis-strong.xlsx
+++ b/study03/report/correlation/effective-participants/SimpleCorrPairAnalysis-strong.xlsx
@@ -6,16 +6,19 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="strong_spearman_25" r:id="rId3" sheetId="1"/>
-    <sheet name="strong_spearman_54" r:id="rId4" sheetId="2"/>
+    <sheet name="strong_spearman_7" r:id="rId3" sheetId="1"/>
+    <sheet name="strong_spearman_25" r:id="rId4" sheetId="2"/>
+    <sheet name="strong_spearman_34" r:id="rId5" sheetId="3"/>
+    <sheet name="strong_spearman_45" r:id="rId6" sheetId="4"/>
+    <sheet name="strong_spearman_70" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="59">
   <si>
-    <t>Correlation information for DiffTheta - Interest/Enjoyment in ont-gamified.Master using the method: spearman</t>
+    <t>Correlation information for Gains in Skills/Knowledge - Intrinsic Motivation in ont-gamified.Master using the method: spearman</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -24,10 +27,10 @@
     <t>Correlation matrix</t>
   </si>
   <si>
-    <t>DiffTheta</t>
+    <t>Gains in Skills/Knowledge</t>
   </si>
   <si>
-    <t>Interest/Enjoyment</t>
+    <t>Intrinsic Motivation</t>
   </si>
   <si>
     <t>Matrix of t-test value</t>
@@ -51,13 +54,13 @@
     <t>p</t>
   </si>
   <si>
-    <t>DffTh-Int/E</t>
+    <t>GiS/K-IntrM</t>
   </si>
   <si>
-    <t>Data source for DiffTheta - Interest/Enjoyment in ont-gamified.Master</t>
+    <t>Data source for Gains in Skills/Knowledge - Intrinsic Motivation in ont-gamified.Master</t>
   </si>
   <si>
-    <t>Data full source for DiffTheta - Interest/Enjoyment in ont-gamified.Master</t>
+    <t>Data full source for Gains in Skills/Knowledge - Intrinsic Motivation in ont-gamified.Master</t>
   </si>
   <si>
     <t>UserID</t>
@@ -81,13 +84,13 @@
     <t>ont-gamified</t>
   </si>
   <si>
-    <t>Warriors</t>
-  </si>
-  <si>
     <t>Outlaws</t>
   </si>
   <si>
     <t>Vandals</t>
+  </si>
+  <si>
+    <t>Vikings</t>
   </si>
   <si>
     <t>Silly Knights</t>
@@ -108,19 +111,49 @@
     <t>Yee Achiever</t>
   </si>
   <si>
-    <t>Correlation information for DiffTheta - Effort/Importance in w/o-gamified.Master using the method: spearman</t>
+    <t>Correlation information for Gains in Skills/Knowledge - Perceived Choice in ont-gamified.Master using the method: spearman</t>
+  </si>
+  <si>
+    <t>Perceived Choice</t>
+  </si>
+  <si>
+    <t>GiS/K-PrcvC</t>
+  </si>
+  <si>
+    <t>Data source for Gains in Skills/Knowledge - Perceived Choice in ont-gamified.Master</t>
+  </si>
+  <si>
+    <t>Data full source for Gains in Skills/Knowledge - Perceived Choice in ont-gamified.Master</t>
+  </si>
+  <si>
+    <t>Correlation information for Gains in Skills/Knowledge - Pressure/Tension in ont-gamified.Master using the method: spearman</t>
+  </si>
+  <si>
+    <t>Pressure/Tension</t>
+  </si>
+  <si>
+    <t>GiS/K-Prs/T</t>
+  </si>
+  <si>
+    <t>Data source for Gains in Skills/Knowledge - Pressure/Tension in ont-gamified.Master</t>
+  </si>
+  <si>
+    <t>Data full source for Gains in Skills/Knowledge - Pressure/Tension in ont-gamified.Master</t>
+  </si>
+  <si>
+    <t>Correlation information for Gains in Skills/Knowledge - Effort/Importance in w/o-gamified.Master using the method: spearman</t>
   </si>
   <si>
     <t>Effort/Importance</t>
   </si>
   <si>
-    <t>DffTh-Eff/I</t>
+    <t>GiS/K-Eff/I</t>
   </si>
   <si>
-    <t>Data source for DiffTheta - Effort/Importance in w/o-gamified.Master</t>
+    <t>Data source for Gains in Skills/Knowledge - Effort/Importance in w/o-gamified.Master</t>
   </si>
   <si>
-    <t>Data full source for DiffTheta - Effort/Importance in w/o-gamified.Master</t>
+    <t>Data full source for Gains in Skills/Knowledge - Effort/Importance in w/o-gamified.Master</t>
   </si>
   <si>
     <t>w/o-gamified</t>
@@ -138,10 +171,28 @@
     <t>Grupo3</t>
   </si>
   <si>
+    <t>Grupo5</t>
+  </si>
+  <si>
     <t>Grupo9</t>
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Correlation information for Gains in Skills/Knowledge - Relevance in ont-gamified.Master using the method: spearman</t>
+  </si>
+  <si>
+    <t>Relevance</t>
+  </si>
+  <si>
+    <t>GiS/K-Rlvnc</t>
+  </si>
+  <si>
+    <t>Data source for Gains in Skills/Knowledge - Relevance in ont-gamified.Master</t>
+  </si>
+  <si>
+    <t>Data full source for Gains in Skills/Knowledge - Relevance in ont-gamified.Master</t>
   </si>
 </sst>
 </file>
@@ -149,13 +200,1432 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="149">
+  <fonts count="371">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="22.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="18.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <i val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1146,7 +2616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="281">
+  <cellXfs count="701">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -1476,6 +2946,498 @@
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="171" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="174" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="181" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="182" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="182" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="182" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="186" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="193" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="195" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="196" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="197" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="198" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="199" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="200" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="201" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="202" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="203" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="204" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="204" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="204" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="205" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="206" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="207" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="208" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="209" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="210" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="211" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="212" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="213" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="214" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="214" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="214" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="215" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="216" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="217" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="218" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="219" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="220" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="221" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="222" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="223" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="224" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="225" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="226" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="227" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="228" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="229" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="230" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="231" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="232" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="233" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="234" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="235" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="236" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="236" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="236" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="237" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="238" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="239" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="240" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="241" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="242" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="243" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="244" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="245" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="246" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="246" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="246" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="247" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="248" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="249" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="250" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="251" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="252" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="253" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="254" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="255" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="256" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="256" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="256" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="257" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="258" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="259" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="260" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="261" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="262" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="263" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="264" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="265" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="266" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="266" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="266" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="267" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="268" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="269" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="270" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="271" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="272" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="273" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="274" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="275" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="276" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="277" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="278" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="278" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="278" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="279" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="280" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="281" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="282" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="283" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="284" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="285" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="286" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="287" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="288" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="288" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="288" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="289" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="290" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="291" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="292" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="293" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="294" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="295" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="296" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="297" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="298" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="299" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="300" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="301" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="302" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="303" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="304" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="305" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="306" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="307" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="308" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="309" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="310" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="310" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="310" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="311" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="312" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="313" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="314" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="315" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="316" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="317" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="318" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="319" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="320" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="320" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="320" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="321" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="322" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="323" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="324" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="325" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="326" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="327" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="328" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="329" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="330" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="330" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="330" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="331" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="332" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="333" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="334" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="335" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="336" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="337" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="338" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="339" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="340" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="340" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="340" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="341" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="342" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="343" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="344" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="345" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="346" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="347" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="348" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="349" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="350" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="351" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="352" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="352" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="352" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="353" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="354" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="355" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="356" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="357" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="358" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="359" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="360" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="361" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="362" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="362" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="362" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="363" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="364" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="365" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="366" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="367" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="368" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="369" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="370" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1536,7 +3498,7 @@
         <v>1.0</v>
       </c>
       <c r="C6" t="n" s="32">
-        <v>-0.8285714285714285</v>
+        <v>0.8285714285714285</v>
       </c>
     </row>
     <row r="7">
@@ -1544,7 +3506,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="n" s="31">
-        <v>-0.8285714285714285</v>
+        <v>0.8285714285714285</v>
       </c>
       <c r="C7" t="n" s="32">
         <v>1.0</v>
@@ -1582,7 +3544,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C12" t="n" s="52">
-        <v>-2.9598001058630063</v>
+        <v>2.9598001058630063</v>
       </c>
     </row>
     <row r="13">
@@ -1590,7 +3552,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="n" s="51">
-        <v>-2.9598001058630063</v>
+        <v>2.9598001058630063</v>
       </c>
       <c r="C13" t="e" s="52">
         <v>#DIV/0!</v>
@@ -1677,13 +3639,13 @@
         <v>12</v>
       </c>
       <c r="B24" t="n" s="91">
-        <v>-0.9806845993491808</v>
+        <v>0.051929318847277625</v>
       </c>
       <c r="C24" t="n" s="92">
-        <v>-0.8285714285714285</v>
+        <v>0.8285714285714285</v>
       </c>
       <c r="D24" t="n" s="93">
-        <v>-0.05192931884727761</v>
+        <v>0.9806845993491808</v>
       </c>
       <c r="E24" t="n" s="94">
         <v>0.04156268221574347</v>
@@ -1714,50 +3676,50 @@
     </row>
     <row r="29">
       <c r="A29" t="n" s="113">
-        <v>0.16957045618326988</v>
+        <v>-0.13718543611105669</v>
       </c>
       <c r="B29" t="n" s="114">
-        <v>0.5136755173037465</v>
+        <v>-0.5032931597030925</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n" s="113">
-        <v>0.056303131700413886</v>
+        <v>0.12005763951268636</v>
       </c>
       <c r="B30" t="n" s="114">
-        <v>0.3072097500789291</v>
+        <v>0.7664435857103108</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n" s="113">
-        <v>0.1057289325304706</v>
+        <v>-0.0767619167297687</v>
       </c>
       <c r="B31" t="n" s="114">
-        <v>-0.5415918102542824</v>
+        <v>0.331895701460983</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n" s="113">
-        <v>0.013932201703524574</v>
+        <v>0.00926342200375345</v>
       </c>
       <c r="B32" t="n" s="114">
-        <v>1.2994045801764238</v>
+        <v>1.25854320906581</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n" s="113">
-        <v>-0.023457684006790103</v>
+        <v>-0.024982259368366677</v>
       </c>
       <c r="B33" t="n" s="114">
-        <v>1.6363701348851551</v>
+        <v>0.285481793014026</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n" s="113">
-        <v>0.05532693638498046</v>
+        <v>-0.16159606382871694</v>
       </c>
       <c r="B34" t="n" s="114">
-        <v>1.1179968928576578</v>
+        <v>0.11834231828023933</v>
       </c>
     </row>
     <row r="35">
@@ -1803,10 +3765,10 @@
     </row>
     <row r="39">
       <c r="A39" t="n" s="133">
-        <v>10175.0</v>
+        <v>10176.0</v>
       </c>
       <c r="B39" t="n" s="134">
-        <v>1.03107E7</v>
+        <v>1.0276949E7</v>
       </c>
       <c r="C39" t="s" s="135">
         <v>21</v>
@@ -1821,18 +3783,18 @@
         <v>29</v>
       </c>
       <c r="G39" t="n" s="139">
-        <v>0.16957045618326988</v>
+        <v>-0.13718543611105669</v>
       </c>
       <c r="H39" t="n" s="140">
-        <v>0.5136755173037465</v>
+        <v>-0.5032931597030925</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n" s="133">
-        <v>10176.0</v>
+        <v>10188.0</v>
       </c>
       <c r="B40" t="n" s="134">
-        <v>1.0276949E7</v>
+        <v>1.0276995E7</v>
       </c>
       <c r="C40" t="s" s="135">
         <v>21</v>
@@ -1844,21 +3806,21 @@
         <v>28</v>
       </c>
       <c r="F40" t="s" s="138">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G40" t="n" s="139">
-        <v>0.056303131700413886</v>
+        <v>0.12005763951268636</v>
       </c>
       <c r="H40" t="n" s="140">
-        <v>0.3072097500789291</v>
+        <v>0.7664435857103108</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n" s="133">
-        <v>10188.0</v>
+        <v>10215.0</v>
       </c>
       <c r="B41" t="n" s="134">
-        <v>1.0276995E7</v>
+        <v>9285227.0</v>
       </c>
       <c r="C41" t="s" s="135">
         <v>21</v>
@@ -1870,13 +3832,13 @@
         <v>28</v>
       </c>
       <c r="F41" t="s" s="138">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G41" t="n" s="139">
-        <v>0.1057289325304706</v>
+        <v>-0.0767619167297687</v>
       </c>
       <c r="H41" t="n" s="140">
-        <v>-0.5415918102542824</v>
+        <v>0.331895701460983</v>
       </c>
     </row>
     <row r="42">
@@ -1899,10 +3861,10 @@
         <v>29</v>
       </c>
       <c r="G42" t="n" s="139">
-        <v>0.013932201703524574</v>
+        <v>0.00926342200375345</v>
       </c>
       <c r="H42" t="n" s="140">
-        <v>1.2994045801764238</v>
+        <v>1.25854320906581</v>
       </c>
     </row>
     <row r="43">
@@ -1925,10 +3887,10 @@
         <v>29</v>
       </c>
       <c r="G43" t="n" s="139">
-        <v>-0.023457684006790103</v>
+        <v>-0.024982259368366677</v>
       </c>
       <c r="H43" t="n" s="140">
-        <v>1.6363701348851551</v>
+        <v>0.285481793014026</v>
       </c>
     </row>
     <row r="44">
@@ -1951,10 +3913,10 @@
         <v>29</v>
       </c>
       <c r="G44" t="n" s="139">
-        <v>0.05532693638498046</v>
+        <v>-0.16159606382871694</v>
       </c>
       <c r="H44" t="n" s="140">
-        <v>1.1179968928576578</v>
+        <v>0.11834231828023933</v>
       </c>
     </row>
   </sheetData>
@@ -2015,10 +3977,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="n" s="171">
-        <v>0.9999999999999998</v>
+        <v>1.0</v>
       </c>
       <c r="C6" t="n" s="172">
-        <v>-0.8999999999999998</v>
+        <v>0.8857142857142858</v>
       </c>
     </row>
     <row r="7">
@@ -2026,10 +3988,10 @@
         <v>32</v>
       </c>
       <c r="B7" t="n" s="171">
-        <v>-0.8999999999999998</v>
+        <v>0.8857142857142858</v>
       </c>
       <c r="C7" t="n" s="172">
-        <v>0.9999999999999998</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
@@ -2060,11 +4022,11 @@
       <c r="A12" t="s" s="186">
         <v>3</v>
       </c>
-      <c r="B12" t="n" s="191">
-        <v>8.21912370089156E7</v>
+      <c r="B12" t="e" s="191">
+        <v>#DIV/0!</v>
       </c>
       <c r="C12" t="n" s="192">
-        <v>-3.576237364075613</v>
+        <v>3.8158362203593157</v>
       </c>
     </row>
     <row r="13">
@@ -2072,10 +4034,10 @@
         <v>32</v>
       </c>
       <c r="B13" t="n" s="191">
-        <v>-3.576237364075613</v>
-      </c>
-      <c r="C13" t="n" s="192">
-        <v>8.21912370089156E7</v>
+        <v>3.8158362203593157</v>
+      </c>
+      <c r="C13" t="e" s="192">
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14">
@@ -2107,10 +4069,10 @@
         <v>3</v>
       </c>
       <c r="B18" t="n" s="211">
-        <v>3.971862410081728E-24</v>
+        <v>-0.0</v>
       </c>
       <c r="C18" t="n" s="212">
-        <v>0.03738607346849877</v>
+        <v>0.018845481049562667</v>
       </c>
     </row>
     <row r="19">
@@ -2118,10 +4080,10 @@
         <v>32</v>
       </c>
       <c r="B19" t="n" s="211">
-        <v>0.03738607346849877</v>
+        <v>0.018845481049562667</v>
       </c>
       <c r="C19" t="n" s="212">
-        <v>3.971862410081728E-24</v>
+        <v>-0.0</v>
       </c>
     </row>
     <row r="20">
@@ -2159,16 +4121,16 @@
         <v>33</v>
       </c>
       <c r="B24" t="n" s="231">
-        <v>-0.9934375159687521</v>
+        <v>0.26371272512610916</v>
       </c>
       <c r="C24" t="n" s="232">
-        <v>-0.8999999999999998</v>
+        <v>0.8857142857142858</v>
       </c>
       <c r="D24" t="n" s="233">
-        <v>-0.08610194023847699</v>
+        <v>0.9874704963803648</v>
       </c>
       <c r="E24" t="n" s="234">
-        <v>0.03738607346849877</v>
+        <v>0.018845481049562667</v>
       </c>
     </row>
     <row r="25">
@@ -2196,47 +4158,50 @@
     </row>
     <row r="29">
       <c r="A29" t="n" s="253">
-        <v>-0.04972506425419933</v>
+        <v>-0.13718543611105669</v>
       </c>
       <c r="B29" t="n" s="254">
-        <v>-0.48044512673196493</v>
+        <v>-0.571541021942381</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n" s="253">
-        <v>-0.09871476844150755</v>
+        <v>0.12005763951268636</v>
       </c>
       <c r="B30" t="n" s="254">
-        <v>1.1239812929970028</v>
+        <v>1.6300613239310544</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n" s="253">
-        <v>-0.10791832418840941</v>
+        <v>-0.0767619167297687</v>
       </c>
       <c r="B31" t="n" s="254">
-        <v>-0.2219491622123673</v>
+        <v>0.9510779812680862</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n" s="253">
-        <v>-0.04705566070438302</v>
+        <v>0.00926342200375345</v>
       </c>
       <c r="B32" t="n" s="254">
-        <v>-2.237469100991422</v>
+        <v>1.2580230179601286</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n" s="253">
-        <v>-0.04935925715204929</v>
+        <v>-0.024982259368366677</v>
       </c>
       <c r="B33" t="n" s="254">
-        <v>-1.0729933441403883</v>
+        <v>0.08661004612576251</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>1</v>
+      <c r="A34" t="n" s="253">
+        <v>-0.16159606382871694</v>
+      </c>
+      <c r="B34" t="n" s="254">
+        <v>-0.07137047387597562</v>
       </c>
     </row>
     <row r="35">
@@ -2245,164 +4210,1641 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s" s="258">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="258">
         <v>35</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="s" s="272">
+    <row r="38">
+      <c r="A38" t="s" s="272">
         <v>15</v>
       </c>
-      <c r="B37" t="s" s="272">
+      <c r="B38" t="s" s="272">
         <v>16</v>
       </c>
-      <c r="C37" t="s" s="272">
+      <c r="C38" t="s" s="272">
         <v>17</v>
       </c>
-      <c r="D37" t="s" s="272">
+      <c r="D38" t="s" s="272">
         <v>18</v>
       </c>
-      <c r="E37" t="s" s="272">
+      <c r="E38" t="s" s="272">
         <v>19</v>
       </c>
-      <c r="F37" t="s" s="272">
+      <c r="F38" t="s" s="272">
         <v>20</v>
       </c>
-      <c r="G37" t="s" s="272">
+      <c r="G38" t="s" s="272">
         <v>3</v>
       </c>
-      <c r="H37" t="s" s="272">
+      <c r="H38" t="s" s="272">
         <v>32</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n" s="273">
-        <v>10174.0</v>
-      </c>
-      <c r="B38" t="n" s="274">
-        <v>1.0276852E7</v>
-      </c>
-      <c r="C38" t="s" s="275">
-        <v>36</v>
-      </c>
-      <c r="D38" t="s" s="276">
-        <v>37</v>
-      </c>
-      <c r="E38" t="s" s="277">
-        <v>28</v>
-      </c>
-      <c r="F38" t="s" s="278">
-        <v>42</v>
-      </c>
-      <c r="G38" t="n" s="279">
-        <v>-0.04972506425419933</v>
-      </c>
-      <c r="H38" t="n" s="280">
-        <v>-0.48044512673196493</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n" s="273">
-        <v>10179.0</v>
+        <v>10176.0</v>
       </c>
       <c r="B39" t="n" s="274">
-        <v>1.0310759E7</v>
+        <v>1.0276949E7</v>
       </c>
       <c r="C39" t="s" s="275">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D39" t="s" s="276">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E39" t="s" s="277">
         <v>28</v>
       </c>
       <c r="F39" t="s" s="278">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G39" t="n" s="279">
-        <v>-0.09871476844150755</v>
+        <v>-0.13718543611105669</v>
       </c>
       <c r="H39" t="n" s="280">
-        <v>1.1239812929970028</v>
+        <v>-0.571541021942381</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n" s="273">
-        <v>10191.0</v>
+        <v>10188.0</v>
       </c>
       <c r="B40" t="n" s="274">
-        <v>1.0276981E7</v>
+        <v>1.0276995E7</v>
       </c>
       <c r="C40" t="s" s="275">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D40" t="s" s="276">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s" s="277">
         <v>28</v>
       </c>
       <c r="F40" t="s" s="278">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G40" t="n" s="279">
-        <v>-0.10791832418840941</v>
+        <v>0.12005763951268636</v>
       </c>
       <c r="H40" t="n" s="280">
-        <v>-0.2219491622123673</v>
+        <v>1.6300613239310544</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n" s="273">
-        <v>10219.0</v>
+        <v>10215.0</v>
       </c>
       <c r="B41" t="n" s="274">
-        <v>1.0276831E7</v>
+        <v>9285227.0</v>
       </c>
       <c r="C41" t="s" s="275">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D41" t="s" s="276">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E41" t="s" s="277">
         <v>28</v>
       </c>
       <c r="F41" t="s" s="278">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G41" t="n" s="279">
-        <v>-0.04705566070438302</v>
+        <v>-0.0767619167297687</v>
       </c>
       <c r="H41" t="n" s="280">
-        <v>-2.237469100991422</v>
+        <v>0.9510779812680862</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n" s="273">
-        <v>10231.0</v>
+        <v>10216.0</v>
       </c>
       <c r="B42" t="n" s="274">
-        <v>1.0276911E7</v>
+        <v>1.027672E7</v>
       </c>
       <c r="C42" t="s" s="275">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D42" t="s" s="276">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E42" t="s" s="277">
         <v>28</v>
       </c>
       <c r="F42" t="s" s="278">
+        <v>29</v>
+      </c>
+      <c r="G42" t="n" s="279">
+        <v>0.00926342200375345</v>
+      </c>
+      <c r="H42" t="n" s="280">
+        <v>1.2580230179601286</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="273">
+        <v>10223.0</v>
+      </c>
+      <c r="B43" t="n" s="274">
+        <v>9795185.0</v>
+      </c>
+      <c r="C43" t="s" s="275">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s" s="276">
+        <v>26</v>
+      </c>
+      <c r="E43" t="s" s="277">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s" s="278">
+        <v>29</v>
+      </c>
+      <c r="G43" t="n" s="279">
+        <v>-0.024982259368366677</v>
+      </c>
+      <c r="H43" t="n" s="280">
+        <v>0.08661004612576251</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n" s="273">
+        <v>10230.0</v>
+      </c>
+      <c r="B44" t="n" s="274">
+        <v>1.0351992E7</v>
+      </c>
+      <c r="C44" t="s" s="275">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s" s="276">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s" s="277">
+        <v>28</v>
+      </c>
+      <c r="F44" t="s" s="278">
+        <v>29</v>
+      </c>
+      <c r="G44" t="n" s="279">
+        <v>-0.16159606382871694</v>
+      </c>
+      <c r="H44" t="n" s="280">
+        <v>-0.07137047387597562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="14.0" customWidth="true"/>
+    <col min="2" max="2" width="14.0" customWidth="true"/>
+    <col min="3" max="3" width="14.0" customWidth="true"/>
+    <col min="4" max="4" width="14.0" customWidth="true"/>
+    <col min="5" max="5" width="14.0" customWidth="true"/>
+    <col min="6" max="6" width="14.0" customWidth="true"/>
+    <col min="7" max="7" width="14.0" customWidth="true"/>
+    <col min="8" max="8" width="14.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="282">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="296">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5" t="s" s="310">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s" s="310">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="306">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n" s="311">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="n" s="312">
+        <v>-0.8696565534786727</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="306">
+        <v>37</v>
+      </c>
+      <c r="B7" t="n" s="311">
+        <v>-0.8696565534786727</v>
+      </c>
+      <c r="C7" t="n" s="312">
+        <v>0.9999999999999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="316">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11" t="s" s="330">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s" s="330">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="326">
+        <v>3</v>
+      </c>
+      <c r="B12" t="e" s="331">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12" t="n" s="332">
+        <v>-3.5233213170882216</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="326">
+        <v>37</v>
+      </c>
+      <c r="B13" t="n" s="331">
+        <v>-3.5233213170882216</v>
+      </c>
+      <c r="C13" t="n" s="332">
+        <v>1.3421772799999999E8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="336">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="s" s="350">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s" s="350">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="346">
+        <v>3</v>
+      </c>
+      <c r="B18" t="n" s="351">
+        <v>-0.0</v>
+      </c>
+      <c r="C18" t="n" s="352">
+        <v>0.0243768916856908</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="346">
+        <v>37</v>
+      </c>
+      <c r="B19" t="n" s="351">
+        <v>0.0243768916856908</v>
+      </c>
+      <c r="C19" t="n" s="352">
+        <v>1.8488927466117675E-32</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="356">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23"/>
+      <c r="B23" t="s" s="370">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s" s="370">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s" s="370">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s" s="370">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="366">
+        <v>38</v>
+      </c>
+      <c r="B24" t="n" s="371">
+        <v>-0.9856008638855045</v>
+      </c>
+      <c r="C24" t="n" s="372">
+        <v>-0.8696565534786727</v>
+      </c>
+      <c r="D24" t="n" s="373">
+        <v>-0.1974549415680596</v>
+      </c>
+      <c r="E24" t="n" s="374">
+        <v>0.0243768916856908</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="378">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="392">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s" s="392">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n" s="393">
+        <v>-0.13718543611105669</v>
+      </c>
+      <c r="B29" t="n" s="394">
+        <v>0.6739289455131704</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n" s="393">
+        <v>0.12005763951268636</v>
+      </c>
+      <c r="B30" t="n" s="394">
+        <v>-1.5713683015865159</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="393">
+        <v>-0.0767619167297687</v>
+      </c>
+      <c r="B31" t="n" s="394">
+        <v>-0.34516387181251634</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n" s="393">
+        <v>0.00926342200375345</v>
+      </c>
+      <c r="B32" t="n" s="394">
+        <v>-1.5713683015865159</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="393">
+        <v>-0.024982259368366677</v>
+      </c>
+      <c r="B33" t="n" s="394">
+        <v>0.09842018285070941</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="393">
+        <v>-0.16159606382871694</v>
+      </c>
+      <c r="B34" t="n" s="394">
+        <v>0.34930127604675565</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="398">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="412">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s" s="412">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s" s="412">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s" s="412">
+        <v>18</v>
+      </c>
+      <c r="E38" t="s" s="412">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s" s="412">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s" s="412">
+        <v>3</v>
+      </c>
+      <c r="H38" t="s" s="412">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="413">
+        <v>10176.0</v>
+      </c>
+      <c r="B39" t="n" s="414">
+        <v>1.0276949E7</v>
+      </c>
+      <c r="C39" t="s" s="415">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s" s="416">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s" s="417">
+        <v>28</v>
+      </c>
+      <c r="F39" t="s" s="418">
+        <v>29</v>
+      </c>
+      <c r="G39" t="n" s="419">
+        <v>-0.13718543611105669</v>
+      </c>
+      <c r="H39" t="n" s="420">
+        <v>0.6739289455131704</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="413">
+        <v>10188.0</v>
+      </c>
+      <c r="B40" t="n" s="414">
+        <v>1.0276995E7</v>
+      </c>
+      <c r="C40" t="s" s="415">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s" s="416">
+        <v>23</v>
+      </c>
+      <c r="E40" t="s" s="417">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s" s="418">
+        <v>30</v>
+      </c>
+      <c r="G40" t="n" s="419">
+        <v>0.12005763951268636</v>
+      </c>
+      <c r="H40" t="n" s="420">
+        <v>-1.5713683015865159</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="413">
+        <v>10215.0</v>
+      </c>
+      <c r="B41" t="n" s="414">
+        <v>9285227.0</v>
+      </c>
+      <c r="C41" t="s" s="415">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s" s="416">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s" s="417">
+        <v>28</v>
+      </c>
+      <c r="F41" t="s" s="418">
+        <v>29</v>
+      </c>
+      <c r="G41" t="n" s="419">
+        <v>-0.0767619167297687</v>
+      </c>
+      <c r="H41" t="n" s="420">
+        <v>-0.34516387181251634</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n" s="413">
+        <v>10216.0</v>
+      </c>
+      <c r="B42" t="n" s="414">
+        <v>1.027672E7</v>
+      </c>
+      <c r="C42" t="s" s="415">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s" s="416">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s" s="417">
+        <v>28</v>
+      </c>
+      <c r="F42" t="s" s="418">
+        <v>29</v>
+      </c>
+      <c r="G42" t="n" s="419">
+        <v>0.00926342200375345</v>
+      </c>
+      <c r="H42" t="n" s="420">
+        <v>-1.5713683015865159</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="413">
+        <v>10223.0</v>
+      </c>
+      <c r="B43" t="n" s="414">
+        <v>9795185.0</v>
+      </c>
+      <c r="C43" t="s" s="415">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s" s="416">
+        <v>26</v>
+      </c>
+      <c r="E43" t="s" s="417">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s" s="418">
+        <v>29</v>
+      </c>
+      <c r="G43" t="n" s="419">
+        <v>-0.024982259368366677</v>
+      </c>
+      <c r="H43" t="n" s="420">
+        <v>0.09842018285070941</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n" s="413">
+        <v>10230.0</v>
+      </c>
+      <c r="B44" t="n" s="414">
+        <v>1.0351992E7</v>
+      </c>
+      <c r="C44" t="s" s="415">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s" s="416">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s" s="417">
+        <v>28</v>
+      </c>
+      <c r="F44" t="s" s="418">
+        <v>29</v>
+      </c>
+      <c r="G44" t="n" s="419">
+        <v>-0.16159606382871694</v>
+      </c>
+      <c r="H44" t="n" s="420">
+        <v>0.34930127604675565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="14.0" customWidth="true"/>
+    <col min="2" max="2" width="14.0" customWidth="true"/>
+    <col min="3" max="3" width="14.0" customWidth="true"/>
+    <col min="4" max="4" width="14.0" customWidth="true"/>
+    <col min="5" max="5" width="14.0" customWidth="true"/>
+    <col min="6" max="6" width="14.0" customWidth="true"/>
+    <col min="7" max="7" width="14.0" customWidth="true"/>
+    <col min="8" max="8" width="14.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="422">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="436">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5" t="s" s="450">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s" s="450">
         <v>42</v>
       </c>
-      <c r="G42" t="n" s="279">
-        <v>-0.04935925715204929</v>
-      </c>
-      <c r="H42" t="n" s="280">
-        <v>-1.0729933441403883</v>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="446">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n" s="451">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="C6" t="n" s="452">
+        <v>-0.753702346348183</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="446">
+        <v>42</v>
+      </c>
+      <c r="B7" t="n" s="451">
+        <v>-0.753702346348183</v>
+      </c>
+      <c r="C7" t="n" s="452">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="456">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11" t="s" s="470">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s" s="470">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="466">
+        <v>3</v>
+      </c>
+      <c r="B12" t="n" s="471">
+        <v>1.3421772799999999E8</v>
+      </c>
+      <c r="C12" t="n" s="472">
+        <v>-2.293621675234401</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="466">
+        <v>42</v>
+      </c>
+      <c r="B13" t="n" s="471">
+        <v>-2.293621675234401</v>
+      </c>
+      <c r="C13" t="e" s="472">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="476">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="s" s="490">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s" s="490">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="486">
+        <v>3</v>
+      </c>
+      <c r="B18" t="n" s="491">
+        <v>1.8488927466117675E-32</v>
+      </c>
+      <c r="C18" t="n" s="492">
+        <v>0.08352328137325986</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="486">
+        <v>42</v>
+      </c>
+      <c r="B19" t="n" s="491">
+        <v>0.08352328137325986</v>
+      </c>
+      <c r="C19" t="n" s="492">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="496">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23"/>
+      <c r="B23" t="s" s="510">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s" s="510">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s" s="510">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s" s="510">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="506">
+        <v>43</v>
+      </c>
+      <c r="B24" t="n" s="511">
+        <v>-0.971202632953137</v>
+      </c>
+      <c r="C24" t="n" s="512">
+        <v>-0.753702346348183</v>
+      </c>
+      <c r="D24" t="n" s="513">
+        <v>0.14899640118872431</v>
+      </c>
+      <c r="E24" t="n" s="514">
+        <v>0.08352328137325986</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="518">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="532">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s" s="532">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n" s="533">
+        <v>-0.06419279982804033</v>
+      </c>
+      <c r="B29" t="n" s="534">
+        <v>-0.48050764026194936</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n" s="533">
+        <v>-0.12975245830274829</v>
+      </c>
+      <c r="B30" t="n" s="534">
+        <v>1.1239667537909057</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="533">
+        <v>-0.12975245830274829</v>
+      </c>
+      <c r="B31" t="n" s="534">
+        <v>-0.22200760025946803</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n" s="533">
+        <v>-0.01644788860766827</v>
+      </c>
+      <c r="B32" t="n" s="534">
+        <v>-2.237659609198312</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="533">
+        <v>-0.06899602363501679</v>
+      </c>
+      <c r="B33" t="n" s="534">
+        <v>-0.7623920958210545</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="533">
+        <v>-0.09113189471052305</v>
+      </c>
+      <c r="B34" t="n" s="534">
+        <v>-1.0730990232837903</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="538">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="552">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s" s="552">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s" s="552">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s" s="552">
+        <v>18</v>
+      </c>
+      <c r="E38" t="s" s="552">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s" s="552">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s" s="552">
+        <v>3</v>
+      </c>
+      <c r="H38" t="s" s="552">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="553">
+        <v>10174.0</v>
+      </c>
+      <c r="B39" t="n" s="554">
+        <v>1.0276852E7</v>
+      </c>
+      <c r="C39" t="s" s="555">
+        <v>46</v>
+      </c>
+      <c r="D39" t="s" s="556">
+        <v>47</v>
+      </c>
+      <c r="E39" t="s" s="557">
+        <v>28</v>
+      </c>
+      <c r="F39" t="s" s="558">
+        <v>53</v>
+      </c>
+      <c r="G39" t="n" s="559">
+        <v>-0.06419279982804033</v>
+      </c>
+      <c r="H39" t="n" s="560">
+        <v>-0.48050764026194936</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="553">
+        <v>10179.0</v>
+      </c>
+      <c r="B40" t="n" s="554">
+        <v>1.0310759E7</v>
+      </c>
+      <c r="C40" t="s" s="555">
+        <v>46</v>
+      </c>
+      <c r="D40" t="s" s="556">
+        <v>48</v>
+      </c>
+      <c r="E40" t="s" s="557">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s" s="558">
+        <v>53</v>
+      </c>
+      <c r="G40" t="n" s="559">
+        <v>-0.12975245830274829</v>
+      </c>
+      <c r="H40" t="n" s="560">
+        <v>1.1239667537909057</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="553">
+        <v>10191.0</v>
+      </c>
+      <c r="B41" t="n" s="554">
+        <v>1.0276981E7</v>
+      </c>
+      <c r="C41" t="s" s="555">
+        <v>46</v>
+      </c>
+      <c r="D41" t="s" s="556">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s" s="557">
+        <v>28</v>
+      </c>
+      <c r="F41" t="s" s="558">
+        <v>53</v>
+      </c>
+      <c r="G41" t="n" s="559">
+        <v>-0.12975245830274829</v>
+      </c>
+      <c r="H41" t="n" s="560">
+        <v>-0.22200760025946803</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n" s="553">
+        <v>10219.0</v>
+      </c>
+      <c r="B42" t="n" s="554">
+        <v>1.0276831E7</v>
+      </c>
+      <c r="C42" t="s" s="555">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s" s="556">
+        <v>50</v>
+      </c>
+      <c r="E42" t="s" s="557">
+        <v>28</v>
+      </c>
+      <c r="F42" t="s" s="558">
+        <v>53</v>
+      </c>
+      <c r="G42" t="n" s="559">
+        <v>-0.01644788860766827</v>
+      </c>
+      <c r="H42" t="n" s="560">
+        <v>-2.237659609198312</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="553">
+        <v>10227.0</v>
+      </c>
+      <c r="B43" t="n" s="554">
+        <v>9274382.0</v>
+      </c>
+      <c r="C43" t="s" s="555">
+        <v>46</v>
+      </c>
+      <c r="D43" t="s" s="556">
+        <v>51</v>
+      </c>
+      <c r="E43" t="s" s="557">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s" s="558">
+        <v>53</v>
+      </c>
+      <c r="G43" t="n" s="559">
+        <v>-0.06899602363501679</v>
+      </c>
+      <c r="H43" t="n" s="560">
+        <v>-0.7623920958210545</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n" s="553">
+        <v>10231.0</v>
+      </c>
+      <c r="B44" t="n" s="554">
+        <v>1.0276911E7</v>
+      </c>
+      <c r="C44" t="s" s="555">
+        <v>46</v>
+      </c>
+      <c r="D44" t="s" s="556">
+        <v>52</v>
+      </c>
+      <c r="E44" t="s" s="557">
+        <v>28</v>
+      </c>
+      <c r="F44" t="s" s="558">
+        <v>53</v>
+      </c>
+      <c r="G44" t="n" s="559">
+        <v>-0.09113189471052305</v>
+      </c>
+      <c r="H44" t="n" s="560">
+        <v>-1.0730990232837903</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="14.0" customWidth="true"/>
+    <col min="2" max="2" width="14.0" customWidth="true"/>
+    <col min="3" max="3" width="14.0" customWidth="true"/>
+    <col min="4" max="4" width="14.0" customWidth="true"/>
+    <col min="5" max="5" width="14.0" customWidth="true"/>
+    <col min="6" max="6" width="14.0" customWidth="true"/>
+    <col min="7" max="7" width="14.0" customWidth="true"/>
+    <col min="8" max="8" width="14.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="562">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="576">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5" t="s" s="590">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s" s="590">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="586">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n" s="591">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="n" s="592">
+        <v>0.7714285714285715</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="586">
+        <v>55</v>
+      </c>
+      <c r="B7" t="n" s="591">
+        <v>0.7714285714285715</v>
+      </c>
+      <c r="C7" t="n" s="592">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="596">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11" t="s" s="610">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s" s="610">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="606">
+        <v>3</v>
+      </c>
+      <c r="B12" t="e" s="611">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12" t="n" s="612">
+        <v>2.4246715773614613</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="606">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n" s="611">
+        <v>2.4246715773614613</v>
+      </c>
+      <c r="C13" t="e" s="612">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="616">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="s" s="630">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s" s="630">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="626">
+        <v>3</v>
+      </c>
+      <c r="B18" t="n" s="631">
+        <v>-0.0</v>
+      </c>
+      <c r="C18" t="n" s="632">
+        <v>0.07239650145772598</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="626">
+        <v>55</v>
+      </c>
+      <c r="B19" t="n" s="631">
+        <v>0.07239650145772598</v>
+      </c>
+      <c r="C19" t="n" s="632">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="636">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23"/>
+      <c r="B23" t="s" s="650">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s" s="650">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s" s="650">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s" s="650">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="646">
+        <v>56</v>
+      </c>
+      <c r="B24" t="n" s="651">
+        <v>-0.1073243682425376</v>
+      </c>
+      <c r="C24" t="n" s="652">
+        <v>0.7714285714285715</v>
+      </c>
+      <c r="D24" t="n" s="653">
+        <v>0.973511637634403</v>
+      </c>
+      <c r="E24" t="n" s="654">
+        <v>0.07239650145772598</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="658">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="672">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s" s="672">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n" s="673">
+        <v>-0.13718543611105669</v>
+      </c>
+      <c r="B29" t="n" s="674">
+        <v>-0.3108569225270983</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n" s="673">
+        <v>0.12005763951268636</v>
+      </c>
+      <c r="B30" t="n" s="674">
+        <v>1.2636388752683616</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="673">
+        <v>-0.0767619167297687</v>
+      </c>
+      <c r="B31" t="n" s="674">
+        <v>1.073618905316245</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n" s="673">
+        <v>0.00926342200375345</v>
+      </c>
+      <c r="B32" t="n" s="674">
+        <v>0.8665603425851527</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="673">
+        <v>-0.024982259368366677</v>
+      </c>
+      <c r="B33" t="n" s="674">
+        <v>0.22500798859924598</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="673">
+        <v>-0.16159606382871694</v>
+      </c>
+      <c r="B34" t="n" s="674">
+        <v>0.07522575398791864</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="678">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="692">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s" s="692">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s" s="692">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s" s="692">
+        <v>18</v>
+      </c>
+      <c r="E38" t="s" s="692">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s" s="692">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s" s="692">
+        <v>3</v>
+      </c>
+      <c r="H38" t="s" s="692">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="693">
+        <v>10176.0</v>
+      </c>
+      <c r="B39" t="n" s="694">
+        <v>1.0276949E7</v>
+      </c>
+      <c r="C39" t="s" s="695">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s" s="696">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s" s="697">
+        <v>28</v>
+      </c>
+      <c r="F39" t="s" s="698">
+        <v>29</v>
+      </c>
+      <c r="G39" t="n" s="699">
+        <v>-0.13718543611105669</v>
+      </c>
+      <c r="H39" t="n" s="700">
+        <v>-0.3108569225270983</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="693">
+        <v>10188.0</v>
+      </c>
+      <c r="B40" t="n" s="694">
+        <v>1.0276995E7</v>
+      </c>
+      <c r="C40" t="s" s="695">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s" s="696">
+        <v>23</v>
+      </c>
+      <c r="E40" t="s" s="697">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s" s="698">
+        <v>30</v>
+      </c>
+      <c r="G40" t="n" s="699">
+        <v>0.12005763951268636</v>
+      </c>
+      <c r="H40" t="n" s="700">
+        <v>1.2636388752683616</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="693">
+        <v>10215.0</v>
+      </c>
+      <c r="B41" t="n" s="694">
+        <v>9285227.0</v>
+      </c>
+      <c r="C41" t="s" s="695">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s" s="696">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s" s="697">
+        <v>28</v>
+      </c>
+      <c r="F41" t="s" s="698">
+        <v>29</v>
+      </c>
+      <c r="G41" t="n" s="699">
+        <v>-0.0767619167297687</v>
+      </c>
+      <c r="H41" t="n" s="700">
+        <v>1.073618905316245</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n" s="693">
+        <v>10216.0</v>
+      </c>
+      <c r="B42" t="n" s="694">
+        <v>1.027672E7</v>
+      </c>
+      <c r="C42" t="s" s="695">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s" s="696">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s" s="697">
+        <v>28</v>
+      </c>
+      <c r="F42" t="s" s="698">
+        <v>29</v>
+      </c>
+      <c r="G42" t="n" s="699">
+        <v>0.00926342200375345</v>
+      </c>
+      <c r="H42" t="n" s="700">
+        <v>0.8665603425851527</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="693">
+        <v>10223.0</v>
+      </c>
+      <c r="B43" t="n" s="694">
+        <v>9795185.0</v>
+      </c>
+      <c r="C43" t="s" s="695">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s" s="696">
+        <v>26</v>
+      </c>
+      <c r="E43" t="s" s="697">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s" s="698">
+        <v>29</v>
+      </c>
+      <c r="G43" t="n" s="699">
+        <v>-0.024982259368366677</v>
+      </c>
+      <c r="H43" t="n" s="700">
+        <v>0.22500798859924598</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n" s="693">
+        <v>10230.0</v>
+      </c>
+      <c r="B44" t="n" s="694">
+        <v>1.0351992E7</v>
+      </c>
+      <c r="C44" t="s" s="695">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s" s="696">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s" s="697">
+        <v>28</v>
+      </c>
+      <c r="F44" t="s" s="698">
+        <v>29</v>
+      </c>
+      <c r="G44" t="n" s="699">
+        <v>-0.16159606382871694</v>
+      </c>
+      <c r="H44" t="n" s="700">
+        <v>0.07522575398791864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>